<commit_message>
feat/ added home page content and more recent rounds
</commit_message>
<xml_diff>
--- a/app/data/Summary_Data.xlsx
+++ b/app/data/Summary_Data.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Summary!$A$1:$I$25</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Summary!$A$1:$I$35</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="36">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t xml:space="preserve">William</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trentham Golf Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tohe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bro’s so cracked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the start of very honest golf. No Gimme’s, no Mulligans no breakfast balls or kick outs Wasn’t really trying here, too pissed off lol</t>
   </si>
 </sst>
 </file>
@@ -436,10 +448,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,7 +460,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="81.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="113.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,7 +1116,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
-        <v>45984</v>
+        <v>45979</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
@@ -1113,25 +1125,26 @@
         <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>48</v>
+        <f aca="false">5+5+4+5+8+5+6+5+7</f>
+        <v>50</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">SUM(F24-G24)</f>
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
-        <v>46002</v>
+        <v>45984</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>16</v>
@@ -1140,23 +1153,20 @@
         <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">SUM(F25-G25)</f>
-        <v>9</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,41 +1186,44 @@
         <v>13</v>
       </c>
       <c r="F26" s="1" t="n">
-        <f aca="false">G26+H26</f>
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G26" s="1" t="n">
         <v>37</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>15</v>
+        <f aca="false">SUM(F26-G26)</f>
+        <v>9</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
-        <v>46039</v>
+        <v>46002</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="1" t="n">
-        <f aca="false">4+5+4+8+4+5+5+4+4</f>
-        <v>43</v>
+        <f aca="false">G27+H27</f>
+        <v>52</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,7 +1234,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -1230,14 +1243,14 @@
         <v>13</v>
       </c>
       <c r="F28" s="1" t="n">
-        <f aca="false">6+6+8+5+6+7+6+5+5</f>
-        <v>54</v>
+        <f aca="false">4+5+4+8+4+5+5+4+4</f>
+        <v>43</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>29</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,7 +1261,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
@@ -1257,48 +1270,216 @@
         <v>13</v>
       </c>
       <c r="F29" s="1" t="n">
+        <f aca="false">6+6+8+5+6+7+6+5+5</f>
+        <v>54</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="n">
+        <v>46039</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="n">
         <f aca="false">8+6+6+6+6+7+5+5+5</f>
         <v>54</v>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="G30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H30" s="1" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="n">
-        <v>45979</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="1" t="n">
-        <f aca="false">5+5+4+5+8+5+6+5+7</f>
-        <v>50</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="H30" s="1" t="n">
-        <f aca="false">SUM(F30-G30)</f>
-        <v>13</v>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="n">
+        <v>46046</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <f aca="false">SUM(F31-G31)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="n">
+        <v>46046</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <f aca="false">SUM(F32-G32)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="n">
+        <v>46046</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <f aca="false">SUM(F33-G33)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="n">
+        <v>46046</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <f aca="false">SUM(F34-G34)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="n">
+        <v>46046</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <f aca="false">SUM(F35-G35)</f>
+        <v>18</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">SUM(5+7+4+4+5+4+6+8+5+5+7+6+5+7+6+6+5+6)</f>
+        <v>101</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <f aca="false">SUM(F36-G36)</f>
+        <v>30</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I25">
-    <sortState ref="A2:I25">
-      <sortCondition ref="A2:A25" customList=""/>
+  <autoFilter ref="A1:I35">
+    <sortState ref="A2:I35">
+      <sortCondition ref="A2:A35" customList=""/>
     </sortState>
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>